<commit_message>
Trying to handle secure and non-secure site
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Browser</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>https://advantageonlineshopping.com/</t>
   </si>
   <si>
     <t>SM-G950F</t>
@@ -280,13 +283,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -588,13 +591,13 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="2" width="9.41796875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="26.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.76171875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.49609375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.3828125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.359375" style="3" bestFit="1" customWidth="1"/>
@@ -637,7 +640,7 @@
         <v>2</v>
       </c>
       <c s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -676,10 +679,10 @@
       <c s="2" t="b">
         <v>1</v>
       </c>
+      <c s="6" t="s">
+        <v>8</v>
+      </c>
       <c s="4" t="s">
-        <v>8</v>
-      </c>
-      <c s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -698,11 +701,11 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="6" t="s">
+        <v>10</v>
+      </c>
       <c s="4" t="s">
-        <v>10</v>
-      </c>
-      <c s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row>
@@ -711,7 +714,7 @@
       </c>
       <c s="1"/>
       <c s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c s="2" t="s">
         <v>17</v>
@@ -722,11 +725,11 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="6" t="s">
+        <v>10</v>
+      </c>
       <c s="4" t="s">
-        <v>10</v>
-      </c>
-      <c s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rolled separate business processes into functios.  Added a .highlight to the Username field.
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -26,12 +26,12 @@
     <t>CHROME</t>
   </si>
   <si>
-    <t>iPhone X</t>
-  </si>
-  <si>
     <t>app_identifier</t>
   </si>
   <si>
+    <t>8f8fe2aa0724ef5979a590d0f755ece53275b32f</t>
+  </si>
+  <si>
     <t>com.hpe.iShopping</t>
   </si>
   <si>
@@ -65,9 +65,6 @@
     <t>advantageonlineshopping.com/</t>
   </si>
   <si>
-    <t>7b4e847f6292ed738e01c5dc5f2eed323ba98af5</t>
-  </si>
-  <si>
     <t>ce031713bc66a70d05</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>https://advantageonlineshopping.com/</t>
+  </si>
+  <si>
+    <t>iPhone 6s</t>
   </si>
   <si>
     <t>SM-G950F</t>
@@ -286,10 +286,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -591,14 +591,14 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="2" width="9.41796875" style="3" customWidth="1"/>
     <col min="3" max="3" width="32.76171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.49609375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.53125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.3828125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.359375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.41796875" style="3" customWidth="1"/>
@@ -614,13 +614,13 @@
         <v>0</v>
       </c>
       <c t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c t="s">
         <v>13</v>
       </c>
       <c t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c t="s">
         <v>12</v>
@@ -640,13 +640,13 @@
         <v>2</v>
       </c>
       <c s="1" t="s">
-        <v>20</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="5"/>
+        <v>19</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="6"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -662,7 +662,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="5"/>
+      <c s="6"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -671,7 +671,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c s="2" t="s">
         <v>5</v>
@@ -679,11 +679,11 @@
       <c s="2" t="b">
         <v>1</v>
       </c>
-      <c s="6" t="s">
+      <c s="5" t="s">
         <v>8</v>
       </c>
       <c s="4" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row>
@@ -693,15 +693,15 @@
       <c s="1"/>
       <c s="1"/>
       <c s="2" t="s">
+        <v>16</v>
+      </c>
+      <c s="2" t="s">
         <v>17</v>
-      </c>
-      <c s="2" t="s">
-        <v>18</v>
       </c>
       <c s="2" t="b">
         <v>0</v>
       </c>
-      <c s="6" t="s">
+      <c s="5" t="s">
         <v>10</v>
       </c>
       <c s="4" t="s">
@@ -714,10 +714,10 @@
       </c>
       <c s="1"/>
       <c s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c s="2" t="s">
         <v>9</v>
@@ -725,7 +725,7 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
-      <c s="6" t="s">
+      <c s="5" t="s">
         <v>10</v>
       </c>
       <c s="4" t="s">

</xml_diff>

<commit_message>
Changed the data file to use more stable devices.
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -29,9 +29,6 @@
     <t>app_identifier</t>
   </si>
   <si>
-    <t>8f8fe2aa0724ef5979a590d0f755ece53275b32f</t>
-  </si>
-  <si>
     <t>com.hpe.iShopping</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
     <t>device_id</t>
   </si>
   <si>
+    <t>ed2ff5276810f2265b87cb2d58acc7b9246aa5c4</t>
+  </si>
+  <si>
     <t>ostype</t>
   </si>
   <si>
@@ -71,13 +71,13 @@
     <t>com.Advantage.aShopping</t>
   </si>
   <si>
+    <t>iPhone 8</t>
+  </si>
+  <si>
     <t>URL</t>
   </si>
   <si>
     <t>https://advantageonlineshopping.com/</t>
-  </si>
-  <si>
-    <t>iPhone 6s</t>
   </si>
   <si>
     <t>SM-G950F</t>
@@ -283,10 +283,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -598,7 +598,7 @@
   <cols>
     <col min="1" max="2" width="9.41796875" style="3" customWidth="1"/>
     <col min="3" max="3" width="32.76171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.53125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.27734375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.3828125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.359375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.41796875" style="3" customWidth="1"/>
@@ -608,28 +608,28 @@
   <sheetData>
     <row customFormat="1">
       <c t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c t="s">
         <v>0</v>
       </c>
       <c t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c t="s">
         <v>3</v>
       </c>
       <c t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c t="s">
         <v>14</v>
       </c>
       <c t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row>
@@ -640,7 +640,7 @@
         <v>2</v>
       </c>
       <c s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -653,7 +653,7 @@
         <v>0</v>
       </c>
       <c s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c s="1" t="s">
         <v>15</v>
@@ -671,65 +671,65 @@
       <c s="1"/>
       <c s="1"/>
       <c s="2" t="s">
+        <v>16</v>
+      </c>
+      <c s="2" t="s">
+        <v>17</v>
+      </c>
+      <c s="2" t="b">
+        <v>0</v>
+      </c>
+      <c s="4" t="s">
+        <v>9</v>
+      </c>
+      <c s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>1</v>
+      </c>
+      <c s="1"/>
+      <c s="1" t="s">
+        <v>20</v>
+      </c>
+      <c s="2" t="s">
+        <v>16</v>
+      </c>
+      <c s="2" t="s">
+        <v>8</v>
+      </c>
+      <c s="2" t="b">
+        <v>0</v>
+      </c>
+      <c s="4" t="s">
+        <v>9</v>
+      </c>
+      <c s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>1</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="2" t="s">
+        <v>13</v>
+      </c>
+      <c s="2" t="s">
         <v>4</v>
-      </c>
-      <c s="2" t="s">
-        <v>5</v>
       </c>
       <c s="2" t="b">
         <v>1</v>
       </c>
+      <c s="4" t="s">
+        <v>7</v>
+      </c>
       <c s="5" t="s">
-        <v>8</v>
-      </c>
-      <c s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>1</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="2" t="s">
-        <v>16</v>
-      </c>
-      <c s="2" t="s">
-        <v>17</v>
-      </c>
-      <c s="2" t="b">
-        <v>0</v>
-      </c>
-      <c s="5" t="s">
-        <v>10</v>
-      </c>
-      <c s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>1</v>
-      </c>
-      <c s="1"/>
-      <c s="1" t="s">
-        <v>19</v>
-      </c>
-      <c s="2" t="s">
-        <v>16</v>
-      </c>
-      <c s="2" t="s">
-        <v>9</v>
-      </c>
-      <c s="2" t="b">
-        <v>0</v>
-      </c>
-      <c s="5" t="s">
-        <v>10</v>
-      </c>
-      <c s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated action name to make it easier to identify which action goes with what script in a multi-test solution
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="Action 1" sheetId="2" r:id="rId2"/>
+    <sheet name="AICrossPlatformAction" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -283,13 +283,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -591,7 +591,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -646,7 +646,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="6"/>
+      <c s="4"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -662,7 +662,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="6"/>
+      <c s="4"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -679,7 +679,7 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
-      <c s="4" t="s">
+      <c s="6" t="s">
         <v>9</v>
       </c>
       <c s="5" t="s">
@@ -703,7 +703,7 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
-      <c s="4" t="s">
+      <c s="6" t="s">
         <v>9</v>
       </c>
       <c s="5" t="s">
@@ -725,7 +725,7 @@
       <c s="2" t="b">
         <v>1</v>
       </c>
-      <c s="4" t="s">
+      <c s="6" t="s">
         <v>7</v>
       </c>
       <c s="5" t="s">

</xml_diff>

<commit_message>
Added code to close down the mobile viewer or the browser (depending on which was opened in the iteration)
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -286,10 +286,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -679,10 +679,10 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="5" t="s">
+        <v>9</v>
+      </c>
       <c s="6" t="s">
-        <v>9</v>
-      </c>
-      <c s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -703,10 +703,10 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="5" t="s">
+        <v>9</v>
+      </c>
       <c s="6" t="s">
-        <v>9</v>
-      </c>
-      <c s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -725,10 +725,10 @@
       <c s="2" t="b">
         <v>1</v>
       </c>
+      <c s="5" t="s">
+        <v>7</v>
+      </c>
       <c s="6" t="s">
-        <v>7</v>
-      </c>
-      <c s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated FutureEnhancements function to reflect that the cleanup functionality has been added.
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -283,13 +283,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -646,7 +646,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="4"/>
+      <c s="5"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -662,7 +662,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="4"/>
+      <c s="5"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -679,10 +679,10 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
-      <c s="5" t="s">
+      <c s="6" t="s">
         <v>9</v>
       </c>
-      <c s="6" t="s">
+      <c s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -703,10 +703,10 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
-      <c s="5" t="s">
+      <c s="6" t="s">
         <v>9</v>
       </c>
-      <c s="6" t="s">
+      <c s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -725,10 +725,10 @@
       <c s="2" t="b">
         <v>1</v>
       </c>
-      <c s="5" t="s">
+      <c s="6" t="s">
         <v>7</v>
       </c>
-      <c s="6" t="s">
+      <c s="4" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated data table to reflect updates in the UFTM device IDs and names.
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -29,6 +29,9 @@
     <t>app_identifier</t>
   </si>
   <si>
+    <t>fd76a9d32fb7cc6eb6284cbcab936bc97dcfce35</t>
+  </si>
+  <si>
     <t>com.hpe.iShopping</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
     <t>IOS</t>
   </si>
   <si>
+    <t>SM-G960F</t>
+  </si>
+  <si>
     <t>MC.Browser</t>
   </si>
   <si>
@@ -56,7 +62,7 @@
     <t>device_id</t>
   </si>
   <si>
-    <t>ed2ff5276810f2265b87cb2d58acc7b9246aa5c4</t>
+    <t>234c19cb26017ece</t>
   </si>
   <si>
     <t>ostype</t>
@@ -65,9 +71,6 @@
     <t>advantageonlineshopping.com/</t>
   </si>
   <si>
-    <t>ce031713bc66a70d05</t>
-  </si>
-  <si>
     <t>com.Advantage.aShopping</t>
   </si>
   <si>
@@ -78,9 +81,6 @@
   </si>
   <si>
     <t>https://advantageonlineshopping.com/</t>
-  </si>
-  <si>
-    <t>SM-G950F</t>
   </si>
 </sst>
 </file>
@@ -283,13 +283,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -591,14 +591,14 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="2" width="9.41796875" style="3" customWidth="1"/>
     <col min="3" max="3" width="32.76171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.27734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.15234375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.3828125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.359375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.41796875" style="3" customWidth="1"/>
@@ -608,29 +608,29 @@
   <sheetData>
     <row customFormat="1">
       <c t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c t="s">
         <v>0</v>
       </c>
       <c t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>3</v>
+      </c>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>16</v>
       </c>
       <c t="s">
         <v>12</v>
       </c>
-      <c t="s">
-        <v>3</v>
-      </c>
-      <c t="s">
-        <v>11</v>
-      </c>
-      <c t="s">
-        <v>14</v>
-      </c>
-      <c t="s">
-        <v>10</v>
-      </c>
     </row>
     <row>
       <c s="1" t="s">
@@ -640,29 +640,29 @@
         <v>2</v>
       </c>
       <c s="1" t="s">
-        <v>20</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="5"/>
+        <v>21</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="4"/>
     </row>
     <row>
       <c s="1" t="s">
         <v>0</v>
       </c>
       <c s="1" t="s">
-        <v>6</v>
-      </c>
-      <c s="1" t="s">
-        <v>15</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="5"/>
+        <v>7</v>
+      </c>
+      <c s="1" t="s">
+        <v>17</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="4"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -671,20 +671,20 @@
       <c s="1"/>
       <c s="1"/>
       <c s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="5" t="s">
+        <v>11</v>
+      </c>
       <c s="6" t="s">
         <v>9</v>
       </c>
-      <c s="4" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row>
       <c s="1" t="s">
@@ -692,23 +692,23 @@
       </c>
       <c s="1"/>
       <c s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="5" t="s">
+        <v>11</v>
+      </c>
       <c s="6" t="s">
         <v>9</v>
       </c>
-      <c s="4" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row>
       <c s="1" t="s">
@@ -717,19 +717,19 @@
       <c s="1"/>
       <c s="1"/>
       <c s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c s="2" t="b">
         <v>1</v>
       </c>
+      <c s="5" t="s">
+        <v>8</v>
+      </c>
       <c s="6" t="s">
-        <v>7</v>
-      </c>
-      <c s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for changes coming in UFT One 15.0.2
</commit_message>
<xml_diff>
--- a/AI Cross Demo/Default.xlsx
+++ b/AI Cross Demo/Default.xlsx
@@ -283,13 +283,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -591,7 +591,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -646,7 +646,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="4"/>
+      <c s="6"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -662,7 +662,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="4"/>
+      <c s="6"/>
     </row>
     <row>
       <c s="1" t="s">
@@ -679,10 +679,10 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="4" t="s">
+        <v>11</v>
+      </c>
       <c s="5" t="s">
-        <v>11</v>
-      </c>
-      <c s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -703,10 +703,10 @@
       <c s="2" t="b">
         <v>0</v>
       </c>
+      <c s="4" t="s">
+        <v>11</v>
+      </c>
       <c s="5" t="s">
-        <v>11</v>
-      </c>
-      <c s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -725,10 +725,10 @@
       <c s="2" t="b">
         <v>1</v>
       </c>
+      <c s="4" t="s">
+        <v>8</v>
+      </c>
       <c s="5" t="s">
-        <v>8</v>
-      </c>
-      <c s="6" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>